<commit_message>
NDEA work based on CSV
</commit_message>
<xml_diff>
--- a/Network_DEA/data.xlsx
+++ b/Network_DEA/data.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hamed/Documents/pyjobs/DEA/Network_DEA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4888FBD2-D177-3C4F-9CD8-699CA6CC8672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF1B426-D74B-BB4A-AACA-6C54AA5209EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16280" xr2:uid="{E065D8AE-D802-864D-A423-9967E8915E3F}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16240" xr2:uid="{E065D8AE-D802-864D-A423-9967E8915E3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="17">
   <si>
     <t>DMU</t>
   </si>
@@ -82,7 +82,10 @@
     <t>y2-I</t>
   </si>
   <si>
-    <t>y3</t>
+    <t>f</t>
+  </si>
+  <si>
+    <t>yf</t>
   </si>
 </sst>
 </file>
@@ -452,7 +455,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -486,7 +489,7 @@
         <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -577,8 +580,8 @@
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="1">
-        <v>3</v>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
@@ -689,8 +692,8 @@
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="1">
-        <v>3</v>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C9" s="1">
         <v>3</v>
@@ -801,8 +804,8 @@
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="1">
-        <v>3</v>
+      <c r="B13" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C13" s="1">
         <v>3</v>
@@ -913,8 +916,8 @@
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="1">
-        <v>3</v>
+      <c r="B17" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C17" s="1">
         <v>5</v>
@@ -1025,8 +1028,8 @@
       <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="1">
-        <v>3</v>
+      <c r="B21" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C21" s="1">
         <v>4</v>

</xml_diff>